<commit_message>
removed ER tags from non-ER templates and non-ER tags
</commit_message>
<xml_diff>
--- a/templates/community/RPTU/RPTU_FS_AlgaeGrowth.xlsx
+++ b/templates/community/RPTU/RPTU_FS_AlgaeGrowth.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\nfdi4plants\SWATE_templates\templates\community\RPTU\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stella Eggels\Documents\GitHub\Swate-templates\templates\community\RPTU\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10FB49A1-E250-4B86-9198-88A294CCCC64}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{701A5D37-7796-488A-84BD-9C0D8CF4E3DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0EF3954B-6C77-46F6-A095-1A73D4FD96C0}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{0EF3954B-6C77-46F6-A095-1A73D4FD96C0}"/>
   </bookViews>
   <sheets>
     <sheet name="AlgaeGrowth" sheetId="1" r:id="rId1"/>
@@ -124,7 +124,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1193" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1190" uniqueCount="215">
   <si>
     <t>Source Name</t>
   </si>
@@ -705,15 +705,6 @@
   </si>
   <si>
     <t>annotationTableSweetSkunk39</t>
-  </si>
-  <si>
-    <t>PRIDE</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/DPBO_1000098</t>
-  </si>
-  <si>
-    <t>DPBO</t>
   </si>
   <si>
     <t>Algae</t>
@@ -1383,9 +1374,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 – 2022-Design">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 – 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1423,7 +1414,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 – 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1529,7 +1520,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 – 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1671,7 +1662,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1747,88 +1738,88 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59A0D40F-2FA9-4C21-A087-3BB23680294D}">
   <dimension ref="A1:BT24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BF1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="BF1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="BO2" sqref="BO2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="36.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="36.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.5546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="31" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="44.5703125" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="56.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="42.140625" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="50.28515625" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="28.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="42.140625" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="50.28515625" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="44.5546875" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="56.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="42.109375" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="50.33203125" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="28.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="42.109375" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="50.33203125" hidden="1" customWidth="1"/>
     <col min="11" max="11" width="36" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="42.140625" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="50.28515625" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="36.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="43.42578125" hidden="1" customWidth="1"/>
-    <col min="16" max="16" width="51.5703125" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="27.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="42.109375" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="50.33203125" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="36.44140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="43.44140625" hidden="1" customWidth="1"/>
+    <col min="16" max="16" width="51.5546875" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="27.109375" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="31" hidden="1" customWidth="1"/>
-    <col min="19" max="19" width="38.140625" hidden="1" customWidth="1"/>
+    <col min="19" max="19" width="38.109375" hidden="1" customWidth="1"/>
     <col min="20" max="20" width="28" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="11" hidden="1" customWidth="1"/>
-    <col min="22" max="22" width="44.28515625" hidden="1" customWidth="1"/>
-    <col min="23" max="23" width="52.42578125" hidden="1" customWidth="1"/>
-    <col min="24" max="24" width="37.42578125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="44.33203125" hidden="1" customWidth="1"/>
+    <col min="23" max="23" width="52.44140625" hidden="1" customWidth="1"/>
+    <col min="24" max="24" width="37.44140625" bestFit="1" customWidth="1"/>
     <col min="25" max="26" width="0" hidden="1" customWidth="1"/>
-    <col min="27" max="27" width="36.28515625" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="39.7109375" hidden="1" customWidth="1"/>
+    <col min="27" max="27" width="36.33203125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="39.6640625" hidden="1" customWidth="1"/>
     <col min="29" max="29" width="11" hidden="1" customWidth="1"/>
     <col min="30" max="30" width="33" hidden="1" customWidth="1"/>
-    <col min="31" max="31" width="30.85546875" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="51.140625" hidden="1" customWidth="1"/>
+    <col min="31" max="31" width="30.88671875" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="51.109375" hidden="1" customWidth="1"/>
     <col min="33" max="33" width="11" hidden="1" customWidth="1"/>
-    <col min="34" max="34" width="32.7109375" hidden="1" customWidth="1"/>
+    <col min="34" max="34" width="32.6640625" hidden="1" customWidth="1"/>
     <col min="35" max="35" width="46" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="33.140625" hidden="1" customWidth="1"/>
+    <col min="36" max="36" width="33.109375" hidden="1" customWidth="1"/>
     <col min="37" max="37" width="11" hidden="1" customWidth="1"/>
-    <col min="38" max="38" width="31.28515625" hidden="1" customWidth="1"/>
+    <col min="38" max="38" width="31.33203125" hidden="1" customWidth="1"/>
     <col min="39" max="39" width="26" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="50.28515625" hidden="1" customWidth="1"/>
-    <col min="41" max="41" width="32.7109375" hidden="1" customWidth="1"/>
-    <col min="42" max="42" width="39.7109375" hidden="1" customWidth="1"/>
-    <col min="43" max="43" width="47.140625" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="40.5703125" hidden="1" customWidth="1"/>
+    <col min="40" max="40" width="50.33203125" hidden="1" customWidth="1"/>
+    <col min="41" max="41" width="32.6640625" hidden="1" customWidth="1"/>
+    <col min="42" max="42" width="39.6640625" hidden="1" customWidth="1"/>
+    <col min="43" max="43" width="47.109375" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="40.5546875" hidden="1" customWidth="1"/>
     <col min="45" max="45" width="11" hidden="1" customWidth="1"/>
-    <col min="46" max="46" width="31.140625" hidden="1" customWidth="1"/>
-    <col min="47" max="47" width="31.140625" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="35.7109375" hidden="1" customWidth="1"/>
+    <col min="46" max="46" width="31.109375" hidden="1" customWidth="1"/>
+    <col min="47" max="47" width="31.109375" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="35.6640625" hidden="1" customWidth="1"/>
     <col min="49" max="49" width="31" hidden="1" customWidth="1"/>
-    <col min="50" max="50" width="38.140625" hidden="1" customWidth="1"/>
-    <col min="51" max="51" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="38.109375" hidden="1" customWidth="1"/>
+    <col min="51" max="51" width="26.88671875" bestFit="1" customWidth="1"/>
     <col min="52" max="52" width="33" hidden="1" customWidth="1"/>
-    <col min="53" max="53" width="50.28515625" hidden="1" customWidth="1"/>
-    <col min="54" max="54" width="30.5703125" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="146.7109375" hidden="1" customWidth="1"/>
-    <col min="56" max="56" width="37.85546875" hidden="1" customWidth="1"/>
+    <col min="53" max="53" width="50.33203125" hidden="1" customWidth="1"/>
+    <col min="54" max="54" width="30.5546875" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="146.6640625" hidden="1" customWidth="1"/>
+    <col min="56" max="56" width="37.88671875" hidden="1" customWidth="1"/>
     <col min="57" max="57" width="32" hidden="1" customWidth="1"/>
-    <col min="58" max="58" width="37.7109375" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="37.6640625" bestFit="1" customWidth="1"/>
     <col min="59" max="59" width="0" hidden="1" customWidth="1"/>
-    <col min="60" max="60" width="48.5703125" hidden="1" customWidth="1"/>
-    <col min="61" max="61" width="37.140625" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="23.42578125" hidden="1" customWidth="1"/>
-    <col min="63" max="63" width="49.140625" hidden="1" customWidth="1"/>
-    <col min="64" max="64" width="36.7109375" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="41.5703125" hidden="1" customWidth="1"/>
-    <col min="66" max="66" width="15.7109375" hidden="1" customWidth="1"/>
-    <col min="67" max="67" width="40.28515625" bestFit="1" customWidth="1"/>
-    <col min="68" max="68" width="42.42578125" hidden="1" customWidth="1"/>
+    <col min="60" max="60" width="48.5546875" hidden="1" customWidth="1"/>
+    <col min="61" max="61" width="37.109375" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="23.44140625" hidden="1" customWidth="1"/>
+    <col min="63" max="63" width="49.109375" hidden="1" customWidth="1"/>
+    <col min="64" max="64" width="36.6640625" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="41.5546875" hidden="1" customWidth="1"/>
+    <col min="66" max="66" width="15.6640625" hidden="1" customWidth="1"/>
+    <col min="67" max="67" width="40.33203125" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="42.44140625" hidden="1" customWidth="1"/>
     <col min="69" max="69" width="0" hidden="1" customWidth="1"/>
-    <col min="70" max="70" width="25.85546875" bestFit="1" customWidth="1"/>
-    <col min="71" max="71" width="32.7109375" hidden="1" customWidth="1"/>
-    <col min="72" max="72" width="39.85546875" hidden="1" customWidth="1"/>
-    <col min="73" max="73" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="74" max="74" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="70" max="70" width="25.88671875" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="32.6640625" hidden="1" customWidth="1"/>
+    <col min="72" max="72" width="39.88671875" hidden="1" customWidth="1"/>
+    <col min="73" max="73" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="20.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2001,7 +1992,7 @@
         <v>56</v>
       </c>
       <c r="BF1" s="3" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="BG1" s="3" t="s">
         <v>57</v>
@@ -2010,7 +2001,7 @@
         <v>58</v>
       </c>
       <c r="BI1" s="3" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="BJ1" s="3" t="s">
         <v>59</v>
@@ -2019,7 +2010,7 @@
         <v>60</v>
       </c>
       <c r="BL1" s="3" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="BM1" s="3" t="s">
         <v>61</v>
@@ -2028,19 +2019,19 @@
         <v>62</v>
       </c>
       <c r="BO1" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="BP1" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="BQ1" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="BR1" s="1" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="2" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>64</v>
       </c>
@@ -2250,7 +2241,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="3" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>96</v>
       </c>
@@ -2460,7 +2451,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="4" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>100</v>
       </c>
@@ -2670,7 +2661,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="5" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>103</v>
       </c>
@@ -2880,7 +2871,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="6" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>105</v>
       </c>
@@ -3092,7 +3083,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="7" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>112</v>
       </c>
@@ -3304,7 +3295,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="8" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>114</v>
       </c>
@@ -3516,7 +3507,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="9" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>116</v>
       </c>
@@ -3728,7 +3719,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="10" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>64</v>
       </c>
@@ -3938,7 +3929,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="11" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>96</v>
       </c>
@@ -4148,7 +4139,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="12" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>100</v>
       </c>
@@ -4358,7 +4349,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="13" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>103</v>
       </c>
@@ -4568,7 +4559,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="14" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>105</v>
       </c>
@@ -4780,7 +4771,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="15" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>112</v>
       </c>
@@ -4992,7 +4983,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="16" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>114</v>
       </c>
@@ -5204,7 +5195,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="17" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>116</v>
       </c>
@@ -5416,7 +5407,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="20" spans="1:70" ht="60" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:70" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A20" s="10" t="s">
         <v>127</v>
       </c>
@@ -5522,7 +5513,7 @@
       <c r="BQ20" s="11"/>
       <c r="BR20" s="17"/>
     </row>
-    <row r="21" spans="1:70" s="23" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:70" s="23" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A21" s="18" t="s">
         <v>128</v>
       </c>
@@ -5706,7 +5697,7 @@
       </c>
       <c r="BR21" s="18"/>
     </row>
-    <row r="22" spans="1:70" s="23" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:70" s="23" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A22" s="24" t="s">
         <v>154</v>
       </c>
@@ -5790,7 +5781,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="24" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:70" x14ac:dyDescent="0.3">
       <c r="O24" s="21" t="s">
         <v>130</v>
       </c>
@@ -5817,17 +5808,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7522EC0B-4508-414D-8D78-D44C69537208}">
   <dimension ref="A1:D27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="35.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="57.140625" customWidth="1"/>
+    <col min="1" max="1" width="35.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="57.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="28" t="s">
         <v>160</v>
       </c>
@@ -5835,7 +5826,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="29" t="s">
         <v>161</v>
       </c>
@@ -5843,7 +5834,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="29" t="s">
         <v>162</v>
       </c>
@@ -5851,7 +5842,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="29" t="s">
         <v>163</v>
       </c>
@@ -5859,7 +5850,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="29" t="s">
         <v>164</v>
       </c>
@@ -5867,7 +5858,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="29" t="s">
         <v>165</v>
       </c>
@@ -5875,71 +5866,65 @@
         <v>192</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="30" t="s">
         <v>166</v>
       </c>
       <c r="B7" s="34"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="29" t="s">
         <v>167</v>
       </c>
-      <c r="B8" s="35" t="s">
-        <v>193</v>
-      </c>
+      <c r="B8" s="35"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="29" t="s">
         <v>168</v>
       </c>
-      <c r="B9" s="33" t="s">
-        <v>194</v>
-      </c>
+      <c r="B9" s="33"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="29" t="s">
         <v>169</v>
       </c>
-      <c r="B10" s="33" t="s">
-        <v>195</v>
-      </c>
+      <c r="B10" s="33"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="30" t="s">
         <v>170</v>
       </c>
       <c r="B11" s="34"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="29" t="s">
         <v>171</v>
       </c>
       <c r="B12" s="35" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="C12" t="s">
+        <v>195</v>
+      </c>
+      <c r="D12" t="s">
         <v>198</v>
       </c>
-      <c r="D12" t="s">
-        <v>201</v>
-      </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="29" t="s">
         <v>172</v>
       </c>
       <c r="B13" s="33" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="C13" t="s">
+        <v>196</v>
+      </c>
+      <c r="D13" t="s">
         <v>199</v>
       </c>
-      <c r="D13" t="s">
-        <v>202</v>
-      </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="29" t="s">
         <v>173</v>
       </c>
@@ -5947,109 +5932,109 @@
         <v>87</v>
       </c>
       <c r="C14" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="D14" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="30" t="s">
         <v>174</v>
       </c>
       <c r="B15" s="34"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="29" t="s">
         <v>175</v>
       </c>
       <c r="B16" s="35" t="s">
+        <v>200</v>
+      </c>
+      <c r="C16" t="s">
         <v>203</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D16" t="s">
         <v>206</v>
       </c>
-      <c r="D16" t="s">
-        <v>209</v>
-      </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="29" t="s">
         <v>176</v>
       </c>
       <c r="B17" s="33" t="s">
+        <v>201</v>
+      </c>
+      <c r="C17" t="s">
         <v>204</v>
       </c>
-      <c r="C17" t="s">
+      <c r="D17" t="s">
         <v>207</v>
       </c>
-      <c r="D17" t="s">
-        <v>210</v>
-      </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="29" t="s">
         <v>177</v>
       </c>
       <c r="B18" s="33"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="29" t="s">
         <v>178</v>
       </c>
       <c r="B19" s="38" t="s">
+        <v>202</v>
+      </c>
+      <c r="C19" s="37" t="s">
         <v>205</v>
       </c>
-      <c r="C19" s="37" t="s">
+      <c r="D19" s="37" t="s">
         <v>208</v>
       </c>
-      <c r="D19" s="37" t="s">
-        <v>211</v>
-      </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="29" t="s">
         <v>179</v>
       </c>
       <c r="B20" s="33"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="29" t="s">
         <v>180</v>
       </c>
       <c r="B21" s="33"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="29" t="s">
         <v>181</v>
       </c>
       <c r="B22" s="33"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="29" t="s">
         <v>182</v>
       </c>
       <c r="B23" s="33"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="29" t="s">
         <v>183</v>
       </c>
       <c r="B24" s="33"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="29" t="s">
         <v>184</v>
       </c>
       <c r="B25" s="33"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="29" t="s">
         <v>185</v>
       </c>
       <c r="B26" s="33"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="31" t="s">
         <v>186</v>
       </c>

</xml_diff>